<commit_message>
add: cpk table to notebook
</commit_message>
<xml_diff>
--- a/data/Rutas_Resumen.xlsx
+++ b/data/Rutas_Resumen.xlsx
@@ -7,8 +7,9 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Rutas" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Rutas_Unidad" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Gastos por Unidad" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Rutas" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Rutas_Unidad" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -426,6 +427,312 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:G11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Unidad</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Litros</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Gasto Combustible</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Costo por litro</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Kms Totales</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Gasto Mantenimiento</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>CPK</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>1823</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>23564859.44</v>
+      </c>
+      <c r="C2" t="n">
+        <v>461196837.92868</v>
+      </c>
+      <c r="D2" t="n">
+        <v>19.56694042857142</v>
+      </c>
+      <c r="E2" t="n">
+        <v>1734208</v>
+      </c>
+      <c r="F2" t="n">
+        <v>50879.31</v>
+      </c>
+      <c r="G2" t="n">
+        <v>265.9702395783435</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>1839</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>19890344.8</v>
+      </c>
+      <c r="C3" t="n">
+        <v>389204913.07396</v>
+      </c>
+      <c r="D3" t="n">
+        <v>19.57580044444443</v>
+      </c>
+      <c r="E3" t="n">
+        <v>1534842</v>
+      </c>
+      <c r="F3" t="n">
+        <v>131218.87</v>
+      </c>
+      <c r="G3" t="n">
+        <v>253.665284077423</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>1885</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>17639860.11</v>
+      </c>
+      <c r="C4" t="n">
+        <v>346288330.362969</v>
+      </c>
+      <c r="D4" t="n">
+        <v>19.61239606451614</v>
+      </c>
+      <c r="E4" t="n">
+        <v>1717121</v>
+      </c>
+      <c r="F4" t="n">
+        <v>10330.47</v>
+      </c>
+      <c r="G4" t="n">
+        <v>201.6740001624632</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>1752</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>20057740.62</v>
+      </c>
+      <c r="C5" t="n">
+        <v>393427926.476439</v>
+      </c>
+      <c r="D5" t="n">
+        <v>19.60499997999999</v>
+      </c>
+      <c r="E5" t="n">
+        <v>2613450</v>
+      </c>
+      <c r="F5" t="n">
+        <v>42203.16</v>
+      </c>
+      <c r="G5" t="n">
+        <v>150.5558283634426</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>1970</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>22033674.95</v>
+      </c>
+      <c r="C6" t="n">
+        <v>436867450.244855</v>
+      </c>
+      <c r="D6" t="n">
+        <v>20.1538869117647</v>
+      </c>
+      <c r="E6" t="n">
+        <v>9793020</v>
+      </c>
+      <c r="F6" t="n">
+        <v>39123.91</v>
+      </c>
+      <c r="G6" t="n">
+        <v>44.61407963578702</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>1903</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>19654148.73</v>
+      </c>
+      <c r="C7" t="n">
+        <v>387318956.4651538</v>
+      </c>
+      <c r="D7" t="n">
+        <v>20.07962663157895</v>
+      </c>
+      <c r="E7" t="n">
+        <v>9165448</v>
+      </c>
+      <c r="F7" t="n">
+        <v>14954.2</v>
+      </c>
+      <c r="G7" t="n">
+        <v>42.2602267412519</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>TT02</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>2754.76</v>
+      </c>
+      <c r="C8" t="n">
+        <v>70508.1924</v>
+      </c>
+      <c r="D8" t="n">
+        <v>25.83625000000001</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" t="n">
+        <v>5792.96</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>DC05</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>665.6900000000001</v>
+      </c>
+      <c r="C9" t="n">
+        <v>12936.40969</v>
+      </c>
+      <c r="D9" t="n">
+        <v>19.433084</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" t="n">
+        <v>99431.19</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>DC04</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>11298</v>
+      </c>
+      <c r="C10" t="n">
+        <v>218873.21652</v>
+      </c>
+      <c r="D10" t="n">
+        <v>19.37274</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" t="n">
+        <v>77044.37000000001</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>DC02</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>1239.52</v>
+      </c>
+      <c r="C11" t="n">
+        <v>24087.69628</v>
+      </c>
+      <c r="D11" t="n">
+        <v>19.433084</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" t="n">
+        <v>81901.66</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -621,7 +928,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>

</xml_diff>

<commit_message>
add: identifier and cpk
</commit_message>
<xml_diff>
--- a/data/Rutas_Resumen.xlsx
+++ b/data/Rutas_Resumen.xlsx
@@ -27966,7 +27966,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -27977,218 +27977,288 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>Posición</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>Ruta</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>kmstotales</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Litros</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Cantidad de viajes</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Eficiencia (km/l)</t>
         </is>
       </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>CPK</t>
+        </is>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
         <is>
           <t>TULTITLAN,EM → SAN QUINTIN,BJ/</t>
         </is>
       </c>
-      <c r="B2" t="n">
+      <c r="C2" t="n">
         <v>1150390</v>
       </c>
-      <c r="C2" t="n">
+      <c r="D2" t="n">
         <v>93533.77</v>
       </c>
-      <c r="D2" t="n">
+      <c r="E2" t="n">
         <v>183</v>
       </c>
-      <c r="E2" t="n">
+      <c r="F2" t="n">
         <v>12.29919418408987</v>
       </c>
+      <c r="G2" t="n">
+        <v>19.31470044841836</v>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
         <is>
           <t>CUAUTITLAN IZCALLI,EM → ESCARCEGA,CP</t>
         </is>
       </c>
-      <c r="B3" t="n">
+      <c r="C3" t="n">
         <v>492369</v>
       </c>
-      <c r="C3" t="n">
+      <c r="D3" t="n">
         <v>40477.51</v>
       </c>
-      <c r="D3" t="n">
+      <c r="E3" t="n">
         <v>123</v>
       </c>
-      <c r="E3" t="n">
+      <c r="F3" t="n">
         <v>12.16401404137754</v>
       </c>
+      <c r="G3" t="n">
+        <v>6.470371847307608</v>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
         <is>
           <t>TULTITLAN,EM → TIJUANA,BJ/</t>
         </is>
       </c>
-      <c r="B4" t="n">
+      <c r="C4" t="n">
         <v>2596925</v>
       </c>
-      <c r="C4" t="n">
+      <c r="D4" t="n">
         <v>214640.26</v>
       </c>
-      <c r="D4" t="n">
+      <c r="E4" t="n">
         <v>508</v>
       </c>
-      <c r="E4" t="n">
+      <c r="F4" t="n">
         <v>12.09896503107106</v>
       </c>
+      <c r="G4" t="n">
+        <v>22.94552710008876</v>
+      </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
         <is>
           <t>CUAUTITLAN IZCALLI,EM → SOLIDARIDAD,QR</t>
         </is>
       </c>
-      <c r="B5" t="n">
+      <c r="C5" t="n">
         <v>419175</v>
       </c>
-      <c r="C5" t="n">
+      <c r="D5" t="n">
         <v>35367.57</v>
       </c>
-      <c r="D5" t="n">
+      <c r="E5" t="n">
         <v>115</v>
       </c>
-      <c r="E5" t="n">
+      <c r="F5" t="n">
         <v>11.85195929491339</v>
       </c>
+      <c r="G5" t="n">
+        <v>6.043426602409495</v>
+      </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
         <is>
           <t>TULTITLAN,EM → MEXICALI,BJ/</t>
         </is>
       </c>
-      <c r="B6" t="n">
+      <c r="C6" t="n">
         <v>354770</v>
       </c>
-      <c r="C6" t="n">
+      <c r="D6" t="n">
         <v>31492.76</v>
       </c>
-      <c r="D6" t="n">
+      <c r="E6" t="n">
         <v>65</v>
       </c>
-      <c r="E6" t="n">
+      <c r="F6" t="n">
         <v>11.26512887406502</v>
       </c>
+      <c r="G6" t="n">
+        <v>23.78267234590579</v>
+      </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
         <is>
           <t>ATIZAPAN DE ZARAGO,EM → CIUDAD JUAREZ,CI</t>
         </is>
       </c>
-      <c r="B7" t="n">
+      <c r="C7" t="n">
         <v>229888</v>
       </c>
-      <c r="C7" t="n">
+      <c r="D7" t="n">
         <v>20553.71</v>
       </c>
-      <c r="D7" t="n">
+      <c r="E7" t="n">
         <v>64</v>
       </c>
-      <c r="E7" t="n">
+      <c r="F7" t="n">
         <v>11.18474474924478</v>
       </c>
+      <c r="G7" t="n">
+        <v>27.8651583241622</v>
+      </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr">
         <is>
           <t>TLALNEPANTLA,EM → SOLIDARIDAD,QR</t>
         </is>
       </c>
-      <c r="B8" t="n">
+      <c r="C8" t="n">
         <v>398130</v>
       </c>
-      <c r="C8" t="n">
+      <c r="D8" t="n">
         <v>35623.36</v>
       </c>
-      <c r="D8" t="n">
+      <c r="E8" t="n">
         <v>115</v>
       </c>
-      <c r="E8" t="n">
+      <c r="F8" t="n">
         <v>11.17609343981028</v>
       </c>
+      <c r="G8" t="n">
+        <v>11.88791422506719</v>
+      </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="inlineStr">
         <is>
           <t>TLAJOMULCO DE ZUNI,JA/Mex → MERIDA,YC/</t>
         </is>
       </c>
-      <c r="B9" t="n">
+      <c r="C9" t="n">
         <v>275977</v>
       </c>
-      <c r="C9" t="n">
+      <c r="D9" t="n">
         <v>24806.17</v>
       </c>
-      <c r="D9" t="n">
+      <c r="E9" t="n">
         <v>71</v>
       </c>
-      <c r="E9" t="n">
+      <c r="F9" t="n">
         <v>11.12533696253795</v>
       </c>
+      <c r="G9" t="n">
+        <v>27.00580232297981</v>
+      </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="inlineStr">
         <is>
           <t>APASEO EL ALTO,GJ → MEXICALI,MX/</t>
         </is>
       </c>
-      <c r="B10" t="n">
+      <c r="C10" t="n">
         <v>439648</v>
       </c>
-      <c r="C10" t="n">
+      <c r="D10" t="n">
         <v>39525.35</v>
       </c>
-      <c r="D10" t="n">
+      <c r="E10" t="n">
         <v>88</v>
       </c>
-      <c r="E10" t="n">
+      <c r="F10" t="n">
         <v>11.12319055998239</v>
       </c>
+      <c r="G10" t="n">
+        <v>7.779807821051387</v>
+      </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="inlineStr">
         <is>
           <t>TLALNEPANTLA,EM → HERMOSILLO,SO</t>
         </is>
       </c>
-      <c r="B11" t="n">
+      <c r="C11" t="n">
         <v>291992</v>
       </c>
-      <c r="C11" t="n">
+      <c r="D11" t="n">
         <v>27127.53</v>
       </c>
-      <c r="D11" t="n">
+      <c r="E11" t="n">
         <v>76</v>
       </c>
-      <c r="E11" t="n">
+      <c r="F11" t="n">
         <v>10.76367807905843</v>
+      </c>
+      <c r="G11" t="n">
+        <v>7.283936170943039</v>
       </c>
     </row>
   </sheetData>
@@ -28202,7 +28272,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -28213,218 +28283,288 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>Posición</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>Ruta</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>kmstotales</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Litros</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Cantidad de viajes</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Eficiencia (km/l)</t>
         </is>
       </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>CPK</t>
+        </is>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
         <is>
           <t>APASEO EL ALTO,GJ → PORCONFIRMAR,NF/MX</t>
         </is>
       </c>
-      <c r="B2" t="n">
+      <c r="C2" t="n">
         <v>51</v>
       </c>
-      <c r="C2" t="n">
+      <c r="D2" t="n">
         <v>14528.34</v>
       </c>
-      <c r="D2" t="n">
+      <c r="E2" t="n">
         <v>51</v>
       </c>
-      <c r="E2" t="n">
+      <c r="F2" t="n">
         <v>0.003510380401339726</v>
       </c>
+      <c r="G2" t="n">
+        <v>26742.72581176471</v>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
         <is>
           <t>CUAUTITLAN,EM/ → CUAUTITLAN,EM/</t>
         </is>
       </c>
-      <c r="B3" t="n">
+      <c r="C3" t="n">
         <v>320</v>
       </c>
-      <c r="C3" t="n">
+      <c r="D3" t="n">
         <v>38710.81</v>
       </c>
-      <c r="D3" t="n">
+      <c r="E3" t="n">
         <v>64</v>
       </c>
-      <c r="E3" t="n">
+      <c r="F3" t="n">
         <v>0.008266424804854252</v>
       </c>
+      <c r="G3" t="n">
+        <v>19118.89281191969</v>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
         <is>
           <t>EL MARQUES,QA → EL MARQUES,QA/Mex</t>
         </is>
       </c>
-      <c r="B4" t="n">
+      <c r="C4" t="n">
         <v>304</v>
       </c>
-      <c r="C4" t="n">
+      <c r="D4" t="n">
         <v>11613.63</v>
       </c>
-      <c r="D4" t="n">
+      <c r="E4" t="n">
         <v>19</v>
       </c>
-      <c r="E4" t="n">
+      <c r="F4" t="n">
         <v>0.02617613958770858</v>
       </c>
+      <c r="G4" t="n">
+        <v>1107.15137569079</v>
+      </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
         <is>
           <t>TULTITLAN,EM → UNKNOWN/</t>
         </is>
       </c>
-      <c r="B5" t="n">
+      <c r="C5" t="n">
         <v>3248</v>
       </c>
-      <c r="C5" t="n">
+      <c r="D5" t="n">
         <v>98880.75</v>
       </c>
-      <c r="D5" t="n">
+      <c r="E5" t="n">
         <v>232</v>
       </c>
-      <c r="E5" t="n">
+      <c r="F5" t="n">
         <v>0.03284764729231928</v>
       </c>
+      <c r="G5" t="n">
+        <v>4570.410677494797</v>
+      </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
         <is>
           <t>TULTITLAN,EM → ECATEPEC DE MORELO,EM/</t>
         </is>
       </c>
-      <c r="B6" t="n">
+      <c r="C6" t="n">
         <v>19890</v>
       </c>
-      <c r="C6" t="n">
+      <c r="D6" t="n">
         <v>595722.6800000001</v>
       </c>
-      <c r="D6" t="n">
+      <c r="E6" t="n">
         <v>1105</v>
       </c>
-      <c r="E6" t="n">
+      <c r="F6" t="n">
         <v>0.03338801873381755</v>
       </c>
+      <c r="G6" t="n">
+        <v>5481.384329607672</v>
+      </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
         <is>
           <t>TUXTLA GUTIERREZ,CH → UNKNOWN/</t>
         </is>
       </c>
-      <c r="B7" t="n">
+      <c r="C7" t="n">
         <v>896</v>
       </c>
-      <c r="C7" t="n">
+      <c r="D7" t="n">
         <v>24726.88</v>
       </c>
-      <c r="D7" t="n">
+      <c r="E7" t="n">
         <v>64</v>
       </c>
-      <c r="E7" t="n">
+      <c r="F7" t="n">
         <v>0.03623586962851763</v>
       </c>
+      <c r="G7" t="n">
+        <v>6157.743728477009</v>
+      </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr">
         <is>
           <t>TLALNEPANTLA,EM → CUAUTITLAN,EM/</t>
         </is>
       </c>
-      <c r="B8" t="n">
+      <c r="C8" t="n">
         <v>780</v>
       </c>
-      <c r="C8" t="n">
+      <c r="D8" t="n">
         <v>21272.69</v>
       </c>
-      <c r="D8" t="n">
+      <c r="E8" t="n">
         <v>39</v>
       </c>
-      <c r="E8" t="n">
+      <c r="F8" t="n">
         <v>0.03666673091179348</v>
       </c>
+      <c r="G8" t="n">
+        <v>6039.604892662821</v>
+      </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="inlineStr">
         <is>
           <t>TLAQUEPAQUE,JA/Mex → TENANCINGO,EM</t>
         </is>
       </c>
-      <c r="B9" t="n">
+      <c r="C9" t="n">
         <v>1144</v>
       </c>
-      <c r="C9" t="n">
+      <c r="D9" t="n">
         <v>28058.58</v>
       </c>
-      <c r="D9" t="n">
+      <c r="E9" t="n">
         <v>52</v>
       </c>
-      <c r="E9" t="n">
+      <c r="F9" t="n">
         <v>0.04077184233842197</v>
       </c>
+      <c r="G9" t="n">
+        <v>2176.151316410839</v>
+      </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="inlineStr">
         <is>
           <t>CUAUTITLAN,EM/ → TLALNEPANTLA,EM</t>
         </is>
       </c>
-      <c r="B10" t="n">
+      <c r="C10" t="n">
         <v>4560</v>
       </c>
-      <c r="C10" t="n">
+      <c r="D10" t="n">
         <v>105526.8</v>
       </c>
-      <c r="D10" t="n">
+      <c r="E10" t="n">
         <v>228</v>
       </c>
-      <c r="E10" t="n">
+      <c r="F10" t="n">
         <v>0.04321177179635884</v>
       </c>
+      <c r="G10" t="n">
+        <v>2645.576421704518</v>
+      </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="inlineStr">
         <is>
           <t>TUXTLA GUTIERREZ,CH → TUXTLA GUTIERREZ,CH/Mex</t>
         </is>
       </c>
-      <c r="B11" t="n">
+      <c r="C11" t="n">
         <v>155893</v>
       </c>
-      <c r="C11" t="n">
+      <c r="D11" t="n">
         <v>3568550.13</v>
       </c>
-      <c r="D11" t="n">
+      <c r="E11" t="n">
         <v>9391</v>
       </c>
-      <c r="E11" t="n">
+      <c r="F11" t="n">
         <v>0.04368524872032553</v>
+      </c>
+      <c r="G11" t="n">
+        <v>4989.200344019353</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: page layout, add:higlight button
</commit_message>
<xml_diff>
--- a/data/Rutas_Resumen.xlsx
+++ b/data/Rutas_Resumen.xlsx
@@ -13,6 +13,8 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="CPK_Ruta" sheetId="4" state="visible" r:id="rId4"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Top 10 Rutas Mas Eficientes" sheetId="5" state="visible" r:id="rId5"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Top 10 Rutas Menos Eficientes" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Top 10 Unidades Más Eficientes" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Top 10 Unidades Menos Eficientes" sheetId="8" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -28570,4 +28572,476 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Unidad</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Kms Totales</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Litros</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Eficiencia (km/l)</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>CPK</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>1665</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>125560</v>
+      </c>
+      <c r="C2" t="n">
+        <v>111846.62</v>
+      </c>
+      <c r="D2" t="n">
+        <v>1.122608801231544</v>
+      </c>
+      <c r="E2" t="n">
+        <v>17.53992595759</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>1670</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>1790</v>
+      </c>
+      <c r="C3" t="n">
+        <v>5152</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.3474378881987578</v>
+      </c>
+      <c r="E3" t="n">
+        <v>89.95270058659219</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>1630</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>96</v>
+      </c>
+      <c r="C4" t="n">
+        <v>288</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E4" t="n">
+        <v>58.11822</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>1640</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>89040</v>
+      </c>
+      <c r="C5" t="n">
+        <v>549960.45</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.161902551356193</v>
+      </c>
+      <c r="E5" t="n">
+        <v>121.0195035190364</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>1628</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>216688</v>
+      </c>
+      <c r="C6" t="n">
+        <v>1412981.28</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.1533551810396243</v>
+      </c>
+      <c r="E6" t="n">
+        <v>128.2657230081223</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>1633</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>1060</v>
+      </c>
+      <c r="C7" t="n">
+        <v>6995.17</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.15153312928778</v>
+      </c>
+      <c r="E7" t="n">
+        <v>127.2760094830189</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>1641</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>80316</v>
+      </c>
+      <c r="C8" t="n">
+        <v>554997.12</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.1447142644632102</v>
+      </c>
+      <c r="E8" t="n">
+        <v>135.570475367334</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>1639</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>147277</v>
+      </c>
+      <c r="C9" t="n">
+        <v>1322791.05</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.1113380680947305</v>
+      </c>
+      <c r="E9" t="n">
+        <v>176.4397602208016</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>1649</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>111056</v>
+      </c>
+      <c r="C10" t="n">
+        <v>1159789.86</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.0957552775983056</v>
+      </c>
+      <c r="E10" t="n">
+        <v>204.0743820347212</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>1635</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>36</v>
+      </c>
+      <c r="C11" t="n">
+        <v>458</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.07860262008733625</v>
+      </c>
+      <c r="E11" t="n">
+        <v>246.4643033333333</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Unidad</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Kms Totales</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Litros</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Eficiencia (km/l)</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>CPK</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>1635</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>36</v>
+      </c>
+      <c r="C2" t="n">
+        <v>458</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.07860262008733625</v>
+      </c>
+      <c r="E2" t="n">
+        <v>246.4643033333333</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>1649</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>111056</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1159789.86</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.0957552775983056</v>
+      </c>
+      <c r="E3" t="n">
+        <v>204.0743820347212</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>1639</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>147277</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1322791.05</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.1113380680947305</v>
+      </c>
+      <c r="E4" t="n">
+        <v>176.4397602208016</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>1641</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>80316</v>
+      </c>
+      <c r="C5" t="n">
+        <v>554997.12</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.1447142644632102</v>
+      </c>
+      <c r="E5" t="n">
+        <v>135.570475367334</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>1633</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>1060</v>
+      </c>
+      <c r="C6" t="n">
+        <v>6995.17</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.15153312928778</v>
+      </c>
+      <c r="E6" t="n">
+        <v>127.2760094830189</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>1628</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>216688</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1412981.28</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.1533551810396243</v>
+      </c>
+      <c r="E7" t="n">
+        <v>128.2657230081223</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>1640</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>89040</v>
+      </c>
+      <c r="C8" t="n">
+        <v>549960.45</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.161902551356193</v>
+      </c>
+      <c r="E8" t="n">
+        <v>121.0195035190364</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>1630</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>96</v>
+      </c>
+      <c r="C9" t="n">
+        <v>288</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E9" t="n">
+        <v>58.11822</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>1670</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>1790</v>
+      </c>
+      <c r="C10" t="n">
+        <v>5152</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.3474378881987578</v>
+      </c>
+      <c r="E10" t="n">
+        <v>89.95270058659219</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>1665</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>125560</v>
+      </c>
+      <c r="C11" t="n">
+        <v>111846.62</v>
+      </c>
+      <c r="D11" t="n">
+        <v>1.122608801231544</v>
+      </c>
+      <c r="E11" t="n">
+        <v>17.53992595759</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fix: costo de peajes
</commit_message>
<xml_diff>
--- a/data/Rutas_Resumen.xlsx
+++ b/data/Rutas_Resumen.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G404"/>
+  <dimension ref="A1:H404"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,6 +476,11 @@
           <t>CPK</t>
         </is>
       </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Total Peajes</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -499,7 +504,10 @@
         <v>106421.26</v>
       </c>
       <c r="G2" t="n">
-        <v>1079.108283410909</v>
+        <v>1091.966828865455</v>
+      </c>
+      <c r="H2" t="n">
+        <v>35361</v>
       </c>
     </row>
     <row r="3">
@@ -526,6 +534,9 @@
       <c r="G3" t="n">
         <v>266.8977573956006</v>
       </c>
+      <c r="H3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -551,6 +562,9 @@
       <c r="G4" t="n">
         <v>265.9702395783435</v>
       </c>
+      <c r="H4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -576,6 +590,9 @@
       <c r="G5" t="n">
         <v>253.665284077423</v>
       </c>
+      <c r="H5" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -601,6 +618,9 @@
       <c r="G6" t="n">
         <v>253.2148823928512</v>
       </c>
+      <c r="H6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -626,6 +646,9 @@
       <c r="G7" t="n">
         <v>246.5845168384801</v>
       </c>
+      <c r="H7" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -651,6 +674,9 @@
       <c r="G8" t="n">
         <v>246.4643033333333</v>
       </c>
+      <c r="H8" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -676,6 +702,9 @@
       <c r="G9" t="n">
         <v>242.3156979441523</v>
       </c>
+      <c r="H9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -701,6 +730,9 @@
       <c r="G10" t="n">
         <v>239.2839160394095</v>
       </c>
+      <c r="H10" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -726,6 +758,9 @@
       <c r="G11" t="n">
         <v>238.8757964627331</v>
       </c>
+      <c r="H11" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -751,6 +786,9 @@
       <c r="G12" t="n">
         <v>224.2283565637217</v>
       </c>
+      <c r="H12" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -776,6 +814,9 @@
       <c r="G13" t="n">
         <v>220.946770931004</v>
       </c>
+      <c r="H13" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -801,6 +842,9 @@
       <c r="G14" t="n">
         <v>207.4991931818182</v>
       </c>
+      <c r="H14" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -826,6 +870,9 @@
       <c r="G15" t="n">
         <v>204.0743820347212</v>
       </c>
+      <c r="H15" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -851,6 +898,9 @@
       <c r="G16" t="n">
         <v>201.6740001624632</v>
       </c>
+      <c r="H16" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -876,6 +926,9 @@
       <c r="G17" t="n">
         <v>194.6831353467688</v>
       </c>
+      <c r="H17" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -901,6 +954,9 @@
       <c r="G18" t="n">
         <v>186.0760908184236</v>
       </c>
+      <c r="H18" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -926,6 +982,9 @@
       <c r="G19" t="n">
         <v>180.9159319802148</v>
       </c>
+      <c r="H19" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -951,6 +1010,9 @@
       <c r="G20" t="n">
         <v>178.8196950663757</v>
       </c>
+      <c r="H20" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -976,6 +1038,9 @@
       <c r="G21" t="n">
         <v>178.1452765472019</v>
       </c>
+      <c r="H21" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1001,6 +1066,9 @@
       <c r="G22" t="n">
         <v>176.4397602208016</v>
       </c>
+      <c r="H22" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1026,6 +1094,9 @@
       <c r="G23" t="n">
         <v>175.6010529493244</v>
       </c>
+      <c r="H23" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1051,6 +1122,9 @@
       <c r="G24" t="n">
         <v>175.5608118163774</v>
       </c>
+      <c r="H24" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1076,6 +1150,9 @@
       <c r="G25" t="n">
         <v>168.8803534986794</v>
       </c>
+      <c r="H25" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1101,6 +1178,9 @@
       <c r="G26" t="n">
         <v>163.7515657109423</v>
       </c>
+      <c r="H26" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1126,6 +1206,9 @@
       <c r="G27" t="n">
         <v>158.3249752666426</v>
       </c>
+      <c r="H27" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1151,6 +1234,9 @@
       <c r="G28" t="n">
         <v>157.8051630298059</v>
       </c>
+      <c r="H28" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1176,6 +1262,9 @@
       <c r="G29" t="n">
         <v>156.8756465657478</v>
       </c>
+      <c r="H29" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1201,6 +1290,9 @@
       <c r="G30" t="n">
         <v>153.8665018054946</v>
       </c>
+      <c r="H30" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1226,6 +1318,9 @@
       <c r="G31" t="n">
         <v>150.5558283634426</v>
       </c>
+      <c r="H31" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1251,6 +1346,9 @@
       <c r="G32" t="n">
         <v>146.5211197830656</v>
       </c>
+      <c r="H32" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -1276,6 +1374,9 @@
       <c r="G33" t="n">
         <v>142.3616124669579</v>
       </c>
+      <c r="H33" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1301,6 +1402,9 @@
       <c r="G34" t="n">
         <v>141.0171153294989</v>
       </c>
+      <c r="H34" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1326,6 +1430,9 @@
       <c r="G35" t="n">
         <v>138.5907966020302</v>
       </c>
+      <c r="H35" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -1351,6 +1458,9 @@
       <c r="G36" t="n">
         <v>135.570475367334</v>
       </c>
+      <c r="H36" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1376,6 +1486,9 @@
       <c r="G37" t="n">
         <v>133.827756545925</v>
       </c>
+      <c r="H37" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1401,6 +1514,9 @@
       <c r="G38" t="n">
         <v>128.2657230081223</v>
       </c>
+      <c r="H38" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1426,6 +1542,9 @@
       <c r="G39" t="n">
         <v>127.2760094830189</v>
       </c>
+      <c r="H39" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -1451,6 +1570,9 @@
       <c r="G40" t="n">
         <v>127.068182355595</v>
       </c>
+      <c r="H40" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -1476,6 +1598,9 @@
       <c r="G41" t="n">
         <v>123.688814237678</v>
       </c>
+      <c r="H41" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -1501,6 +1626,9 @@
       <c r="G42" t="n">
         <v>122.7415794223539</v>
       </c>
+      <c r="H42" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -1526,6 +1654,9 @@
       <c r="G43" t="n">
         <v>121.0195035190364</v>
       </c>
+      <c r="H43" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -1551,6 +1682,9 @@
       <c r="G44" t="n">
         <v>114.1414290042495</v>
       </c>
+      <c r="H44" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -1576,6 +1710,9 @@
       <c r="G45" t="n">
         <v>111.8501261128489</v>
       </c>
+      <c r="H45" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -1601,6 +1738,9 @@
       <c r="G46" t="n">
         <v>110.4396877282374</v>
       </c>
+      <c r="H46" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -1626,6 +1766,9 @@
       <c r="G47" t="n">
         <v>109.1771721913989</v>
       </c>
+      <c r="H47" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -1651,6 +1794,9 @@
       <c r="G48" t="n">
         <v>108.9595963679972</v>
       </c>
+      <c r="H48" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -1676,6 +1822,9 @@
       <c r="G49" t="n">
         <v>108.3844886435148</v>
       </c>
+      <c r="H49" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -1701,6 +1850,9 @@
       <c r="G50" t="n">
         <v>102.0600034324434</v>
       </c>
+      <c r="H50" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -1726,6 +1878,9 @@
       <c r="G51" t="n">
         <v>100.7707905913511</v>
       </c>
+      <c r="H51" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -1751,6 +1906,9 @@
       <c r="G52" t="n">
         <v>99.16801260468021</v>
       </c>
+      <c r="H52" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -1776,6 +1934,9 @@
       <c r="G53" t="n">
         <v>99.0106750342068</v>
       </c>
+      <c r="H53" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -1801,6 +1962,9 @@
       <c r="G54" t="n">
         <v>98.95985712185183</v>
       </c>
+      <c r="H54" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -1826,6 +1990,9 @@
       <c r="G55" t="n">
         <v>93.81844948987472</v>
       </c>
+      <c r="H55" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -1851,6 +2018,9 @@
       <c r="G56" t="n">
         <v>92.00640495219531</v>
       </c>
+      <c r="H56" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -1876,6 +2046,9 @@
       <c r="G57" t="n">
         <v>91.58550113411883</v>
       </c>
+      <c r="H57" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -1901,6 +2074,9 @@
       <c r="G58" t="n">
         <v>89.95270058659219</v>
       </c>
+      <c r="H58" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -1926,6 +2102,9 @@
       <c r="G59" t="n">
         <v>88.35861528253157</v>
       </c>
+      <c r="H59" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -1951,6 +2130,9 @@
       <c r="G60" t="n">
         <v>87.90608448213979</v>
       </c>
+      <c r="H60" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -1974,7 +2156,10 @@
         <v>47194.41999999999</v>
       </c>
       <c r="G61" t="n">
-        <v>80.76092471999999</v>
+        <v>80.9619541317647</v>
+      </c>
+      <c r="H61" t="n">
+        <v>1367</v>
       </c>
     </row>
     <row r="62">
@@ -2001,6 +2186,9 @@
       <c r="G62" t="n">
         <v>78.88157631811679</v>
       </c>
+      <c r="H62" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -2026,6 +2214,9 @@
       <c r="G63" t="n">
         <v>78.77262987632849</v>
       </c>
+      <c r="H63" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -2051,6 +2242,9 @@
       <c r="G64" t="n">
         <v>76.36369093744449</v>
       </c>
+      <c r="H64" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -2076,6 +2270,9 @@
       <c r="G65" t="n">
         <v>73.34080700732356</v>
       </c>
+      <c r="H65" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -2101,6 +2298,9 @@
       <c r="G66" t="n">
         <v>72.77680421959697</v>
       </c>
+      <c r="H66" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -2126,6 +2326,9 @@
       <c r="G67" t="n">
         <v>64.22896792173046</v>
       </c>
+      <c r="H67" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -2151,6 +2354,9 @@
       <c r="G68" t="n">
         <v>64.13432462406016</v>
       </c>
+      <c r="H68" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -2176,6 +2382,9 @@
       <c r="G69" t="n">
         <v>60.91511031868531</v>
       </c>
+      <c r="H69" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -2201,6 +2410,9 @@
       <c r="G70" t="n">
         <v>60.27397429146783</v>
       </c>
+      <c r="H70" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -2226,6 +2438,9 @@
       <c r="G71" t="n">
         <v>58.11822</v>
       </c>
+      <c r="H71" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -2251,6 +2466,9 @@
       <c r="G72" t="n">
         <v>57.16393329081906</v>
       </c>
+      <c r="H72" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -2276,6 +2494,9 @@
       <c r="G73" t="n">
         <v>55.73570479300522</v>
       </c>
+      <c r="H73" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -2301,6 +2522,9 @@
       <c r="G74" t="n">
         <v>53.34804823990898</v>
       </c>
+      <c r="H74" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -2326,6 +2550,9 @@
       <c r="G75" t="n">
         <v>52.80791876815101</v>
       </c>
+      <c r="H75" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -2351,6 +2578,9 @@
       <c r="G76" t="n">
         <v>52.63811398189924</v>
       </c>
+      <c r="H76" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -2376,6 +2606,9 @@
       <c r="G77" t="n">
         <v>51.74681078511454</v>
       </c>
+      <c r="H77" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -2401,6 +2634,9 @@
       <c r="G78" t="n">
         <v>49.01452926163277</v>
       </c>
+      <c r="H78" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -2426,6 +2662,9 @@
       <c r="G79" t="n">
         <v>48.10397454197266</v>
       </c>
+      <c r="H79" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -2451,6 +2690,9 @@
       <c r="G80" t="n">
         <v>47.17637729295393</v>
       </c>
+      <c r="H80" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -2476,6 +2718,9 @@
       <c r="G81" t="n">
         <v>44.61407963578702</v>
       </c>
+      <c r="H81" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -2501,6 +2746,9 @@
       <c r="G82" t="n">
         <v>44.59800170590427</v>
       </c>
+      <c r="H82" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -2526,6 +2774,9 @@
       <c r="G83" t="n">
         <v>43.53703150866192</v>
       </c>
+      <c r="H83" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -2551,6 +2802,9 @@
       <c r="G84" t="n">
         <v>42.2602267412519</v>
       </c>
+      <c r="H84" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -2576,6 +2830,9 @@
       <c r="G85" t="n">
         <v>41.38083534361041</v>
       </c>
+      <c r="H85" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -2601,6 +2858,9 @@
       <c r="G86" t="n">
         <v>41.37362325137265</v>
       </c>
+      <c r="H86" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -2626,6 +2886,9 @@
       <c r="G87" t="n">
         <v>41.28818458922477</v>
       </c>
+      <c r="H87" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -2651,6 +2914,9 @@
       <c r="G88" t="n">
         <v>39.89753658013536</v>
       </c>
+      <c r="H88" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -2676,6 +2942,9 @@
       <c r="G89" t="n">
         <v>37.29266801446911</v>
       </c>
+      <c r="H89" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -2701,6 +2970,9 @@
       <c r="G90" t="n">
         <v>36.98627260282164</v>
       </c>
+      <c r="H90" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -2726,6 +2998,9 @@
       <c r="G91" t="n">
         <v>36.74611732025664</v>
       </c>
+      <c r="H91" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -2751,6 +3026,9 @@
       <c r="G92" t="n">
         <v>36.41520363009743</v>
       </c>
+      <c r="H92" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -2776,6 +3054,9 @@
       <c r="G93" t="n">
         <v>36.11086711475633</v>
       </c>
+      <c r="H93" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -2801,6 +3082,9 @@
       <c r="G94" t="n">
         <v>35.64453979911179</v>
       </c>
+      <c r="H94" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -2826,6 +3110,9 @@
       <c r="G95" t="n">
         <v>35.62097530949445</v>
       </c>
+      <c r="H95" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -2851,6 +3138,9 @@
       <c r="G96" t="n">
         <v>35.44282234684941</v>
       </c>
+      <c r="H96" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -2876,6 +3166,9 @@
       <c r="G97" t="n">
         <v>35.28141305797411</v>
       </c>
+      <c r="H97" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -2901,6 +3194,9 @@
       <c r="G98" t="n">
         <v>34.92788375705614</v>
       </c>
+      <c r="H98" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -2926,6 +3222,9 @@
       <c r="G99" t="n">
         <v>34.63111810688044</v>
       </c>
+      <c r="H99" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -2951,6 +3250,9 @@
       <c r="G100" t="n">
         <v>34.62302950806034</v>
       </c>
+      <c r="H100" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -2976,6 +3278,9 @@
       <c r="G101" t="n">
         <v>31.86206127862097</v>
       </c>
+      <c r="H101" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -3001,6 +3306,9 @@
       <c r="G102" t="n">
         <v>31.74108921282761</v>
       </c>
+      <c r="H102" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -3026,6 +3334,9 @@
       <c r="G103" t="n">
         <v>31.61792770462521</v>
       </c>
+      <c r="H103" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -3051,6 +3362,9 @@
       <c r="G104" t="n">
         <v>31.58080520646233</v>
       </c>
+      <c r="H104" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -3076,6 +3390,9 @@
       <c r="G105" t="n">
         <v>31.45958775771534</v>
       </c>
+      <c r="H105" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -3101,6 +3418,9 @@
       <c r="G106" t="n">
         <v>31.3508409401181</v>
       </c>
+      <c r="H106" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -3126,6 +3446,9 @@
       <c r="G107" t="n">
         <v>30.5258306146978</v>
       </c>
+      <c r="H107" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -3151,6 +3474,9 @@
       <c r="G108" t="n">
         <v>30.04885744642161</v>
       </c>
+      <c r="H108" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
@@ -3176,6 +3502,9 @@
       <c r="G109" t="n">
         <v>30.00136939964873</v>
       </c>
+      <c r="H109" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -3201,6 +3530,9 @@
       <c r="G110" t="n">
         <v>29.69609078551655</v>
       </c>
+      <c r="H110" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
@@ -3226,6 +3558,9 @@
       <c r="G111" t="n">
         <v>29.02714925001373</v>
       </c>
+      <c r="H111" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
@@ -3251,6 +3586,9 @@
       <c r="G112" t="n">
         <v>28.81879205114255</v>
       </c>
+      <c r="H112" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
@@ -3276,6 +3614,9 @@
       <c r="G113" t="n">
         <v>28.27828843169643</v>
       </c>
+      <c r="H113" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
@@ -3301,6 +3642,9 @@
       <c r="G114" t="n">
         <v>28.08323123384205</v>
       </c>
+      <c r="H114" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
@@ -3326,6 +3670,9 @@
       <c r="G115" t="n">
         <v>27.58308622821815</v>
       </c>
+      <c r="H115" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
@@ -3351,6 +3698,9 @@
       <c r="G116" t="n">
         <v>27.5026432442269</v>
       </c>
+      <c r="H116" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
@@ -3376,6 +3726,9 @@
       <c r="G117" t="n">
         <v>26.81280270319634</v>
       </c>
+      <c r="H117" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
@@ -3401,6 +3754,9 @@
       <c r="G118" t="n">
         <v>26.61313591220274</v>
       </c>
+      <c r="H118" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
@@ -3426,6 +3782,9 @@
       <c r="G119" t="n">
         <v>26.49746432300307</v>
       </c>
+      <c r="H119" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
@@ -3451,6 +3810,9 @@
       <c r="G120" t="n">
         <v>26.19846975164629</v>
       </c>
+      <c r="H120" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
@@ -3476,6 +3838,9 @@
       <c r="G121" t="n">
         <v>26.17733484902476</v>
       </c>
+      <c r="H121" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
@@ -3501,6 +3866,9 @@
       <c r="G122" t="n">
         <v>24.99389565269359</v>
       </c>
+      <c r="H122" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
@@ -3526,6 +3894,9 @@
       <c r="G123" t="n">
         <v>24.87151241176656</v>
       </c>
+      <c r="H123" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
@@ -3551,6 +3922,9 @@
       <c r="G124" t="n">
         <v>23.89512236720357</v>
       </c>
+      <c r="H124" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
@@ -3576,6 +3950,9 @@
       <c r="G125" t="n">
         <v>23.68413483109111</v>
       </c>
+      <c r="H125" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
@@ -3601,6 +3978,9 @@
       <c r="G126" t="n">
         <v>23.65638112551747</v>
       </c>
+      <c r="H126" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
@@ -3626,6 +4006,9 @@
       <c r="G127" t="n">
         <v>23.34361323966261</v>
       </c>
+      <c r="H127" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
@@ -3651,6 +4034,9 @@
       <c r="G128" t="n">
         <v>22.76195592202613</v>
       </c>
+      <c r="H128" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
@@ -3676,6 +4062,9 @@
       <c r="G129" t="n">
         <v>22.48223457078216</v>
       </c>
+      <c r="H129" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
@@ -3701,6 +4090,9 @@
       <c r="G130" t="n">
         <v>21.75811155858844</v>
       </c>
+      <c r="H130" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
@@ -3726,6 +4118,9 @@
       <c r="G131" t="n">
         <v>21.02636121664688</v>
       </c>
+      <c r="H131" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
@@ -3751,6 +4146,9 @@
       <c r="G132" t="n">
         <v>20.75608563386232</v>
       </c>
+      <c r="H132" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
@@ -3776,6 +4174,9 @@
       <c r="G133" t="n">
         <v>20.7516231179156</v>
       </c>
+      <c r="H133" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
@@ -3801,6 +4202,9 @@
       <c r="G134" t="n">
         <v>20.52540850893407</v>
       </c>
+      <c r="H134" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
@@ -3826,6 +4230,9 @@
       <c r="G135" t="n">
         <v>19.95092477499252</v>
       </c>
+      <c r="H135" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
@@ -3851,6 +4258,9 @@
       <c r="G136" t="n">
         <v>19.76757961171672</v>
       </c>
+      <c r="H136" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
@@ -3876,6 +4286,9 @@
       <c r="G137" t="n">
         <v>19.60670424462946</v>
       </c>
+      <c r="H137" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
@@ -3901,6 +4314,9 @@
       <c r="G138" t="n">
         <v>19.59502677588675</v>
       </c>
+      <c r="H138" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
@@ -3926,6 +4342,9 @@
       <c r="G139" t="n">
         <v>19.4773253948832</v>
       </c>
+      <c r="H139" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
@@ -3951,6 +4370,9 @@
       <c r="G140" t="n">
         <v>19.43412727199168</v>
       </c>
+      <c r="H140" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
@@ -3976,6 +4398,9 @@
       <c r="G141" t="n">
         <v>19.33519219276398</v>
       </c>
+      <c r="H141" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
@@ -4001,6 +4426,9 @@
       <c r="G142" t="n">
         <v>19.32248354103627</v>
       </c>
+      <c r="H142" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
@@ -4026,6 +4454,9 @@
       <c r="G143" t="n">
         <v>19.08583106403103</v>
       </c>
+      <c r="H143" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
@@ -4051,6 +4482,9 @@
       <c r="G144" t="n">
         <v>18.99346474153268</v>
       </c>
+      <c r="H144" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
@@ -4076,6 +4510,9 @@
       <c r="G145" t="n">
         <v>18.90223804946146</v>
       </c>
+      <c r="H145" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
@@ -4101,6 +4538,9 @@
       <c r="G146" t="n">
         <v>18.87987058202357</v>
       </c>
+      <c r="H146" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
@@ -4126,6 +4566,9 @@
       <c r="G147" t="n">
         <v>18.65143027313172</v>
       </c>
+      <c r="H147" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
@@ -4151,6 +4594,9 @@
       <c r="G148" t="n">
         <v>18.46693606622998</v>
       </c>
+      <c r="H148" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
@@ -4176,6 +4622,9 @@
       <c r="G149" t="n">
         <v>18.0460236534768</v>
       </c>
+      <c r="H149" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
@@ -4201,6 +4650,9 @@
       <c r="G150" t="n">
         <v>17.62196112316148</v>
       </c>
+      <c r="H150" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
@@ -4226,6 +4678,9 @@
       <c r="G151" t="n">
         <v>17.53992595759</v>
       </c>
+      <c r="H151" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
@@ -4251,6 +4706,9 @@
       <c r="G152" t="n">
         <v>17.46075268609034</v>
       </c>
+      <c r="H152" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
@@ -4276,6 +4734,9 @@
       <c r="G153" t="n">
         <v>17.1592035246124</v>
       </c>
+      <c r="H153" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
@@ -4301,6 +4762,9 @@
       <c r="G154" t="n">
         <v>17.09954632261469</v>
       </c>
+      <c r="H154" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
@@ -4326,6 +4790,9 @@
       <c r="G155" t="n">
         <v>17.09703525818228</v>
       </c>
+      <c r="H155" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
@@ -4351,6 +4818,9 @@
       <c r="G156" t="n">
         <v>17.00836786098911</v>
       </c>
+      <c r="H156" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
@@ -4376,6 +4846,9 @@
       <c r="G157" t="n">
         <v>17.00598390704171</v>
       </c>
+      <c r="H157" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
@@ -4401,6 +4874,9 @@
       <c r="G158" t="n">
         <v>16.86143328566649</v>
       </c>
+      <c r="H158" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
@@ -4426,6 +4902,9 @@
       <c r="G159" t="n">
         <v>16.52378332453312</v>
       </c>
+      <c r="H159" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
@@ -4451,6 +4930,9 @@
       <c r="G160" t="n">
         <v>16.34051571301456</v>
       </c>
+      <c r="H160" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
@@ -4476,6 +4958,9 @@
       <c r="G161" t="n">
         <v>16.24223093116099</v>
       </c>
+      <c r="H161" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
@@ -4501,6 +4986,9 @@
       <c r="G162" t="n">
         <v>16.1241393079602</v>
       </c>
+      <c r="H162" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
@@ -4526,6 +5014,9 @@
       <c r="G163" t="n">
         <v>16.02778465481771</v>
       </c>
+      <c r="H163" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
@@ -4551,6 +5042,9 @@
       <c r="G164" t="n">
         <v>16.00950545036501</v>
       </c>
+      <c r="H164" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
@@ -4576,6 +5070,9 @@
       <c r="G165" t="n">
         <v>15.94931191054712</v>
       </c>
+      <c r="H165" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
@@ -4601,6 +5098,9 @@
       <c r="G166" t="n">
         <v>15.92962724909879</v>
       </c>
+      <c r="H166" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
@@ -4626,6 +5126,9 @@
       <c r="G167" t="n">
         <v>15.87184386915251</v>
       </c>
+      <c r="H167" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
@@ -4651,6 +5154,9 @@
       <c r="G168" t="n">
         <v>15.83594220767557</v>
       </c>
+      <c r="H168" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
@@ -4676,6 +5182,9 @@
       <c r="G169" t="n">
         <v>15.77459795627824</v>
       </c>
+      <c r="H169" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
@@ -4701,6 +5210,9 @@
       <c r="G170" t="n">
         <v>15.72815419914388</v>
       </c>
+      <c r="H170" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
@@ -4726,6 +5238,9 @@
       <c r="G171" t="n">
         <v>15.71458644057921</v>
       </c>
+      <c r="H171" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
@@ -4751,6 +5266,9 @@
       <c r="G172" t="n">
         <v>15.68107186966292</v>
       </c>
+      <c r="H172" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
@@ -4776,6 +5294,9 @@
       <c r="G173" t="n">
         <v>15.63017349939213</v>
       </c>
+      <c r="H173" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
@@ -4801,6 +5322,9 @@
       <c r="G174" t="n">
         <v>15.54278389554369</v>
       </c>
+      <c r="H174" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
@@ -4826,6 +5350,9 @@
       <c r="G175" t="n">
         <v>15.52149448652833</v>
       </c>
+      <c r="H175" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
@@ -4851,6 +5378,9 @@
       <c r="G176" t="n">
         <v>15.42076972244468</v>
       </c>
+      <c r="H176" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
@@ -4876,6 +5406,9 @@
       <c r="G177" t="n">
         <v>15.25083723099415</v>
       </c>
+      <c r="H177" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
@@ -4901,6 +5434,9 @@
       <c r="G178" t="n">
         <v>15.18845295026968</v>
       </c>
+      <c r="H178" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
@@ -4926,6 +5462,9 @@
       <c r="G179" t="n">
         <v>15.06288147155082</v>
       </c>
+      <c r="H179" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
@@ -4951,6 +5490,9 @@
       <c r="G180" t="n">
         <v>15.04248010290634</v>
       </c>
+      <c r="H180" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
@@ -4976,6 +5518,9 @@
       <c r="G181" t="n">
         <v>15.02456806381113</v>
       </c>
+      <c r="H181" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
@@ -5001,6 +5546,9 @@
       <c r="G182" t="n">
         <v>14.98927663313008</v>
       </c>
+      <c r="H182" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
@@ -5026,6 +5574,9 @@
       <c r="G183" t="n">
         <v>14.96103227029057</v>
       </c>
+      <c r="H183" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
@@ -5051,6 +5602,9 @@
       <c r="G184" t="n">
         <v>14.92672549223853</v>
       </c>
+      <c r="H184" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
@@ -5076,6 +5630,9 @@
       <c r="G185" t="n">
         <v>14.92513303954641</v>
       </c>
+      <c r="H185" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
@@ -5101,6 +5658,9 @@
       <c r="G186" t="n">
         <v>14.86749024557421</v>
       </c>
+      <c r="H186" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
@@ -5126,6 +5686,9 @@
       <c r="G187" t="n">
         <v>14.79393989174646</v>
       </c>
+      <c r="H187" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
@@ -5151,6 +5714,9 @@
       <c r="G188" t="n">
         <v>14.77616301945261</v>
       </c>
+      <c r="H188" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
@@ -5176,6 +5742,9 @@
       <c r="G189" t="n">
         <v>14.73527182841459</v>
       </c>
+      <c r="H189" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
@@ -5201,6 +5770,9 @@
       <c r="G190" t="n">
         <v>14.7085323602851</v>
       </c>
+      <c r="H190" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
@@ -5226,6 +5798,9 @@
       <c r="G191" t="n">
         <v>14.69727452786304</v>
       </c>
+      <c r="H191" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
@@ -5251,6 +5826,9 @@
       <c r="G192" t="n">
         <v>14.52517719620668</v>
       </c>
+      <c r="H192" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr">
@@ -5276,6 +5854,9 @@
       <c r="G193" t="n">
         <v>14.33982266036479</v>
       </c>
+      <c r="H193" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
@@ -5301,6 +5882,9 @@
       <c r="G194" t="n">
         <v>14.27476555479475</v>
       </c>
+      <c r="H194" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
@@ -5326,6 +5910,9 @@
       <c r="G195" t="n">
         <v>14.10410961259016</v>
       </c>
+      <c r="H195" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
@@ -5351,6 +5938,9 @@
       <c r="G196" t="n">
         <v>14.10187324010413</v>
       </c>
+      <c r="H196" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
@@ -5376,6 +5966,9 @@
       <c r="G197" t="n">
         <v>13.97285381101631</v>
       </c>
+      <c r="H197" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="198">
       <c r="A198" t="inlineStr">
@@ -5401,6 +5994,9 @@
       <c r="G198" t="n">
         <v>13.91401063923467</v>
       </c>
+      <c r="H198" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="199">
       <c r="A199" t="inlineStr">
@@ -5426,6 +6022,9 @@
       <c r="G199" t="n">
         <v>13.78505090215689</v>
       </c>
+      <c r="H199" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="200">
       <c r="A200" t="inlineStr">
@@ -5451,6 +6050,9 @@
       <c r="G200" t="n">
         <v>13.75569310871085</v>
       </c>
+      <c r="H200" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="201">
       <c r="A201" t="inlineStr">
@@ -5476,6 +6078,9 @@
       <c r="G201" t="n">
         <v>13.57152971355091</v>
       </c>
+      <c r="H201" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="202">
       <c r="A202" t="inlineStr">
@@ -5501,6 +6106,9 @@
       <c r="G202" t="n">
         <v>13.55516871173207</v>
       </c>
+      <c r="H202" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="203">
       <c r="A203" t="inlineStr">
@@ -5526,6 +6134,9 @@
       <c r="G203" t="n">
         <v>13.39426545143879</v>
       </c>
+      <c r="H203" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="204">
       <c r="A204" t="inlineStr">
@@ -5551,6 +6162,9 @@
       <c r="G204" t="n">
         <v>13.38063536573127</v>
       </c>
+      <c r="H204" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="205">
       <c r="A205" t="inlineStr">
@@ -5576,6 +6190,9 @@
       <c r="G205" t="n">
         <v>13.33197560584176</v>
       </c>
+      <c r="H205" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="206">
       <c r="A206" t="inlineStr">
@@ -5601,6 +6218,9 @@
       <c r="G206" t="n">
         <v>13.33136002232606</v>
       </c>
+      <c r="H206" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="207">
       <c r="A207" t="inlineStr">
@@ -5626,6 +6246,9 @@
       <c r="G207" t="n">
         <v>13.32300952442581</v>
       </c>
+      <c r="H207" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="208">
       <c r="A208" t="inlineStr">
@@ -5651,6 +6274,9 @@
       <c r="G208" t="n">
         <v>13.30872213559198</v>
       </c>
+      <c r="H208" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="209">
       <c r="A209" t="inlineStr">
@@ -5676,6 +6302,9 @@
       <c r="G209" t="n">
         <v>13.26143410081546</v>
       </c>
+      <c r="H209" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="210">
       <c r="A210" t="inlineStr">
@@ -5701,6 +6330,9 @@
       <c r="G210" t="n">
         <v>13.07417037130937</v>
       </c>
+      <c r="H210" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="211">
       <c r="A211" t="inlineStr">
@@ -5726,6 +6358,9 @@
       <c r="G211" t="n">
         <v>13.06336406249183</v>
       </c>
+      <c r="H211" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="212">
       <c r="A212" t="inlineStr">
@@ -5751,6 +6386,9 @@
       <c r="G212" t="n">
         <v>13.04736141649794</v>
       </c>
+      <c r="H212" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="213">
       <c r="A213" t="inlineStr">
@@ -5776,6 +6414,9 @@
       <c r="G213" t="n">
         <v>13.0434668707852</v>
       </c>
+      <c r="H213" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="214">
       <c r="A214" t="inlineStr">
@@ -5801,6 +6442,9 @@
       <c r="G214" t="n">
         <v>12.96648657931271</v>
       </c>
+      <c r="H214" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="215">
       <c r="A215" t="inlineStr">
@@ -5826,6 +6470,9 @@
       <c r="G215" t="n">
         <v>12.86001156152901</v>
       </c>
+      <c r="H215" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="216">
       <c r="A216" t="inlineStr">
@@ -5851,6 +6498,9 @@
       <c r="G216" t="n">
         <v>12.81782040014833</v>
       </c>
+      <c r="H216" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="217">
       <c r="A217" t="inlineStr">
@@ -5876,6 +6526,9 @@
       <c r="G217" t="n">
         <v>12.74604762742059</v>
       </c>
+      <c r="H217" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="218">
       <c r="A218" t="inlineStr">
@@ -5901,6 +6554,9 @@
       <c r="G218" t="n">
         <v>12.70754696715852</v>
       </c>
+      <c r="H218" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="219">
       <c r="A219" t="inlineStr">
@@ -5926,6 +6582,9 @@
       <c r="G219" t="n">
         <v>12.63257288031562</v>
       </c>
+      <c r="H219" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="220">
       <c r="A220" t="inlineStr">
@@ -5951,6 +6610,9 @@
       <c r="G220" t="n">
         <v>12.60575247694665</v>
       </c>
+      <c r="H220" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="221">
       <c r="A221" t="inlineStr">
@@ -5976,6 +6638,9 @@
       <c r="G221" t="n">
         <v>12.51900760162019</v>
       </c>
+      <c r="H221" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="222">
       <c r="A222" t="inlineStr">
@@ -6001,6 +6666,9 @@
       <c r="G222" t="n">
         <v>12.49773192287172</v>
       </c>
+      <c r="H222" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="223">
       <c r="A223" t="inlineStr">
@@ -6026,6 +6694,9 @@
       <c r="G223" t="n">
         <v>12.49210178583146</v>
       </c>
+      <c r="H223" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="224">
       <c r="A224" t="inlineStr">
@@ -6051,6 +6722,9 @@
       <c r="G224" t="n">
         <v>12.46633772755492</v>
       </c>
+      <c r="H224" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="225">
       <c r="A225" t="inlineStr">
@@ -6076,6 +6750,9 @@
       <c r="G225" t="n">
         <v>12.45404053705648</v>
       </c>
+      <c r="H225" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="226">
       <c r="A226" t="inlineStr">
@@ -6101,6 +6778,9 @@
       <c r="G226" t="n">
         <v>12.39959300010101</v>
       </c>
+      <c r="H226" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="227">
       <c r="A227" t="inlineStr">
@@ -6126,6 +6806,9 @@
       <c r="G227" t="n">
         <v>12.39731423396591</v>
       </c>
+      <c r="H227" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="228">
       <c r="A228" t="inlineStr">
@@ -6151,6 +6834,9 @@
       <c r="G228" t="n">
         <v>12.37506684585617</v>
       </c>
+      <c r="H228" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="229">
       <c r="A229" t="inlineStr">
@@ -6176,6 +6862,9 @@
       <c r="G229" t="n">
         <v>12.19445560528062</v>
       </c>
+      <c r="H229" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="230">
       <c r="A230" t="inlineStr">
@@ -6201,6 +6890,9 @@
       <c r="G230" t="n">
         <v>12.18596746666772</v>
       </c>
+      <c r="H230" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="231">
       <c r="A231" t="inlineStr">
@@ -6226,6 +6918,9 @@
       <c r="G231" t="n">
         <v>12.09043913896431</v>
       </c>
+      <c r="H231" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="232">
       <c r="A232" t="inlineStr">
@@ -6251,6 +6946,9 @@
       <c r="G232" t="n">
         <v>12.00631887334661</v>
       </c>
+      <c r="H232" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="233">
       <c r="A233" t="inlineStr">
@@ -6276,6 +6974,9 @@
       <c r="G233" t="n">
         <v>11.95084588553328</v>
       </c>
+      <c r="H233" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="234">
       <c r="A234" t="inlineStr">
@@ -6301,6 +7002,9 @@
       <c r="G234" t="n">
         <v>11.93235974084141</v>
       </c>
+      <c r="H234" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="235">
       <c r="A235" t="inlineStr">
@@ -6326,6 +7030,9 @@
       <c r="G235" t="n">
         <v>11.93196695168847</v>
       </c>
+      <c r="H235" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="236">
       <c r="A236" t="inlineStr">
@@ -6351,6 +7058,9 @@
       <c r="G236" t="n">
         <v>11.82418084580185</v>
       </c>
+      <c r="H236" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="237">
       <c r="A237" t="inlineStr">
@@ -6376,6 +7086,9 @@
       <c r="G237" t="n">
         <v>11.82383291739473</v>
       </c>
+      <c r="H237" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="238">
       <c r="A238" t="inlineStr">
@@ -6401,6 +7114,9 @@
       <c r="G238" t="n">
         <v>11.62968765923945</v>
       </c>
+      <c r="H238" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="239">
       <c r="A239" t="inlineStr">
@@ -6426,6 +7142,9 @@
       <c r="G239" t="n">
         <v>11.61019237834457</v>
       </c>
+      <c r="H239" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="240">
       <c r="A240" t="inlineStr">
@@ -6451,6 +7170,9 @@
       <c r="G240" t="n">
         <v>11.56842292319169</v>
       </c>
+      <c r="H240" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="241">
       <c r="A241" t="inlineStr">
@@ -6476,6 +7198,9 @@
       <c r="G241" t="n">
         <v>11.39844793195021</v>
       </c>
+      <c r="H241" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="242">
       <c r="A242" t="inlineStr">
@@ -6501,6 +7226,9 @@
       <c r="G242" t="n">
         <v>11.38847990799943</v>
       </c>
+      <c r="H242" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="243">
       <c r="A243" t="inlineStr">
@@ -6526,6 +7254,9 @@
       <c r="G243" t="n">
         <v>11.37959940938302</v>
       </c>
+      <c r="H243" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="244">
       <c r="A244" t="inlineStr">
@@ -6551,6 +7282,9 @@
       <c r="G244" t="n">
         <v>11.31741234242102</v>
       </c>
+      <c r="H244" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="245">
       <c r="A245" t="inlineStr">
@@ -6576,6 +7310,9 @@
       <c r="G245" t="n">
         <v>11.30091761247132</v>
       </c>
+      <c r="H245" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="246">
       <c r="A246" t="inlineStr">
@@ -6601,6 +7338,9 @@
       <c r="G246" t="n">
         <v>11.2585738321815</v>
       </c>
+      <c r="H246" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="247">
       <c r="A247" t="inlineStr">
@@ -6626,6 +7366,9 @@
       <c r="G247" t="n">
         <v>11.22538817084678</v>
       </c>
+      <c r="H247" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="248">
       <c r="A248" t="inlineStr">
@@ -6651,6 +7394,9 @@
       <c r="G248" t="n">
         <v>11.1415766292991</v>
       </c>
+      <c r="H248" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="249">
       <c r="A249" t="inlineStr">
@@ -6676,6 +7422,9 @@
       <c r="G249" t="n">
         <v>11.06224070993769</v>
       </c>
+      <c r="H249" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="250">
       <c r="A250" t="inlineStr">
@@ -6701,6 +7450,9 @@
       <c r="G250" t="n">
         <v>11.01453489685538</v>
       </c>
+      <c r="H250" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="251">
       <c r="A251" t="inlineStr">
@@ -6726,6 +7478,9 @@
       <c r="G251" t="n">
         <v>10.85620533556391</v>
       </c>
+      <c r="H251" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="252">
       <c r="A252" t="inlineStr">
@@ -6751,6 +7506,9 @@
       <c r="G252" t="n">
         <v>10.83091960654688</v>
       </c>
+      <c r="H252" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="253">
       <c r="A253" t="inlineStr">
@@ -6776,6 +7534,9 @@
       <c r="G253" t="n">
         <v>10.82716166338583</v>
       </c>
+      <c r="H253" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="254">
       <c r="A254" t="inlineStr">
@@ -6801,6 +7562,9 @@
       <c r="G254" t="n">
         <v>10.799931731593</v>
       </c>
+      <c r="H254" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="255">
       <c r="A255" t="inlineStr">
@@ -6826,6 +7590,9 @@
       <c r="G255" t="n">
         <v>10.77840486455474</v>
       </c>
+      <c r="H255" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="256">
       <c r="A256" t="inlineStr">
@@ -6851,6 +7618,9 @@
       <c r="G256" t="n">
         <v>10.67351047058823</v>
       </c>
+      <c r="H256" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="257">
       <c r="A257" t="inlineStr">
@@ -6876,6 +7646,9 @@
       <c r="G257" t="n">
         <v>10.63649830595005</v>
       </c>
+      <c r="H257" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="258">
       <c r="A258" t="inlineStr">
@@ -6901,6 +7674,9 @@
       <c r="G258" t="n">
         <v>10.53259816334975</v>
       </c>
+      <c r="H258" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="259">
       <c r="A259" t="inlineStr">
@@ -6926,6 +7702,9 @@
       <c r="G259" t="n">
         <v>10.52249382634187</v>
       </c>
+      <c r="H259" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="260">
       <c r="A260" t="inlineStr">
@@ -6951,6 +7730,9 @@
       <c r="G260" t="n">
         <v>10.44803500643819</v>
       </c>
+      <c r="H260" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="261">
       <c r="A261" t="inlineStr">
@@ -6976,6 +7758,9 @@
       <c r="G261" t="n">
         <v>10.42279673602136</v>
       </c>
+      <c r="H261" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="262">
       <c r="A262" t="inlineStr">
@@ -7001,6 +7786,9 @@
       <c r="G262" t="n">
         <v>10.33724564536117</v>
       </c>
+      <c r="H262" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="263">
       <c r="A263" t="inlineStr">
@@ -7026,6 +7814,9 @@
       <c r="G263" t="n">
         <v>10.31618606331739</v>
       </c>
+      <c r="H263" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="264">
       <c r="A264" t="inlineStr">
@@ -7051,6 +7842,9 @@
       <c r="G264" t="n">
         <v>10.23090178305592</v>
       </c>
+      <c r="H264" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="265">
       <c r="A265" t="inlineStr">
@@ -7076,6 +7870,9 @@
       <c r="G265" t="n">
         <v>10.16851171246</v>
       </c>
+      <c r="H265" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="266">
       <c r="A266" t="inlineStr">
@@ -7101,6 +7898,9 @@
       <c r="G266" t="n">
         <v>10.07375652952549</v>
       </c>
+      <c r="H266" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="267">
       <c r="A267" t="inlineStr">
@@ -7126,6 +7926,9 @@
       <c r="G267" t="n">
         <v>10.05535307858502</v>
       </c>
+      <c r="H267" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="268">
       <c r="A268" t="inlineStr">
@@ -7151,6 +7954,9 @@
       <c r="G268" t="n">
         <v>9.936953426703518</v>
       </c>
+      <c r="H268" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="269">
       <c r="A269" t="inlineStr">
@@ -7176,6 +7982,9 @@
       <c r="G269" t="n">
         <v>9.911082221024186</v>
       </c>
+      <c r="H269" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="270">
       <c r="A270" t="inlineStr">
@@ -7201,6 +8010,9 @@
       <c r="G270" t="n">
         <v>9.711043977604227</v>
       </c>
+      <c r="H270" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="271">
       <c r="A271" t="inlineStr">
@@ -7226,6 +8038,9 @@
       <c r="G271" t="n">
         <v>9.678886876304452</v>
       </c>
+      <c r="H271" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="272">
       <c r="A272" t="inlineStr">
@@ -7251,6 +8066,9 @@
       <c r="G272" t="n">
         <v>9.547250531828675</v>
       </c>
+      <c r="H272" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="273">
       <c r="A273" t="inlineStr">
@@ -7276,6 +8094,9 @@
       <c r="G273" t="n">
         <v>9.545666745274943</v>
       </c>
+      <c r="H273" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="274">
       <c r="A274" t="inlineStr">
@@ -7301,6 +8122,9 @@
       <c r="G274" t="n">
         <v>9.492337702900002</v>
       </c>
+      <c r="H274" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="275">
       <c r="A275" t="inlineStr">
@@ -7326,6 +8150,9 @@
       <c r="G275" t="n">
         <v>9.437653574016554</v>
       </c>
+      <c r="H275" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="276">
       <c r="A276" t="inlineStr">
@@ -7351,6 +8178,9 @@
       <c r="G276" t="n">
         <v>9.424423316792556</v>
       </c>
+      <c r="H276" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="277">
       <c r="A277" t="inlineStr">
@@ -7376,6 +8206,9 @@
       <c r="G277" t="n">
         <v>9.412583190732779</v>
       </c>
+      <c r="H277" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="278">
       <c r="A278" t="inlineStr">
@@ -7401,6 +8234,9 @@
       <c r="G278" t="n">
         <v>9.39942528702508</v>
       </c>
+      <c r="H278" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="279">
       <c r="A279" t="inlineStr">
@@ -7426,6 +8262,9 @@
       <c r="G279" t="n">
         <v>9.252674036627841</v>
       </c>
+      <c r="H279" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="280">
       <c r="A280" t="inlineStr">
@@ -7451,6 +8290,9 @@
       <c r="G280" t="n">
         <v>9.236832572749801</v>
       </c>
+      <c r="H280" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="281">
       <c r="A281" t="inlineStr">
@@ -7476,6 +8318,9 @@
       <c r="G281" t="n">
         <v>9.227739394384155</v>
       </c>
+      <c r="H281" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="282">
       <c r="A282" t="inlineStr">
@@ -7501,6 +8346,9 @@
       <c r="G282" t="n">
         <v>9.003320570573527</v>
       </c>
+      <c r="H282" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="283">
       <c r="A283" t="inlineStr">
@@ -7526,6 +8374,9 @@
       <c r="G283" t="n">
         <v>8.940633425012361</v>
       </c>
+      <c r="H283" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="284">
       <c r="A284" t="inlineStr">
@@ -7551,6 +8402,9 @@
       <c r="G284" t="n">
         <v>8.91234379917644</v>
       </c>
+      <c r="H284" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="285">
       <c r="A285" t="inlineStr">
@@ -7576,6 +8430,9 @@
       <c r="G285" t="n">
         <v>8.88586097523541</v>
       </c>
+      <c r="H285" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="286">
       <c r="A286" t="inlineStr">
@@ -7601,6 +8458,9 @@
       <c r="G286" t="n">
         <v>8.725594748559754</v>
       </c>
+      <c r="H286" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="287">
       <c r="A287" t="inlineStr">
@@ -7626,6 +8486,9 @@
       <c r="G287" t="n">
         <v>8.724271892726705</v>
       </c>
+      <c r="H287" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="288">
       <c r="A288" t="inlineStr">
@@ -7651,6 +8514,9 @@
       <c r="G288" t="n">
         <v>8.716539590020719</v>
       </c>
+      <c r="H288" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="289">
       <c r="A289" t="inlineStr">
@@ -7676,6 +8542,9 @@
       <c r="G289" t="n">
         <v>8.696768855106127</v>
       </c>
+      <c r="H289" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="290">
       <c r="A290" t="inlineStr">
@@ -7701,6 +8570,9 @@
       <c r="G290" t="n">
         <v>8.684116954624077</v>
       </c>
+      <c r="H290" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="291">
       <c r="A291" t="inlineStr">
@@ -7726,6 +8598,9 @@
       <c r="G291" t="n">
         <v>8.64853512317857</v>
       </c>
+      <c r="H291" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="292">
       <c r="A292" t="inlineStr">
@@ -7751,6 +8626,9 @@
       <c r="G292" t="n">
         <v>8.639516402202466</v>
       </c>
+      <c r="H292" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="293">
       <c r="A293" t="inlineStr">
@@ -7776,6 +8654,9 @@
       <c r="G293" t="n">
         <v>8.613014139575524</v>
       </c>
+      <c r="H293" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="294">
       <c r="A294" t="inlineStr">
@@ -7801,6 +8682,9 @@
       <c r="G294" t="n">
         <v>8.604592675366865</v>
       </c>
+      <c r="H294" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="295">
       <c r="A295" t="inlineStr">
@@ -7826,6 +8710,9 @@
       <c r="G295" t="n">
         <v>8.466656811969756</v>
       </c>
+      <c r="H295" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="296">
       <c r="A296" t="inlineStr">
@@ -7851,6 +8738,9 @@
       <c r="G296" t="n">
         <v>8.397315823177681</v>
       </c>
+      <c r="H296" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="297">
       <c r="A297" t="inlineStr">
@@ -7876,6 +8766,9 @@
       <c r="G297" t="n">
         <v>8.35971522592118</v>
       </c>
+      <c r="H297" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="298">
       <c r="A298" t="inlineStr">
@@ -7901,6 +8794,9 @@
       <c r="G298" t="n">
         <v>8.325209174910118</v>
       </c>
+      <c r="H298" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="299">
       <c r="A299" t="inlineStr">
@@ -7926,6 +8822,9 @@
       <c r="G299" t="n">
         <v>8.317377482317838</v>
       </c>
+      <c r="H299" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="300">
       <c r="A300" t="inlineStr">
@@ -7951,6 +8850,9 @@
       <c r="G300" t="n">
         <v>8.299377483696485</v>
       </c>
+      <c r="H300" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="301">
       <c r="A301" t="inlineStr">
@@ -7976,6 +8878,9 @@
       <c r="G301" t="n">
         <v>8.060880875359318</v>
       </c>
+      <c r="H301" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="302">
       <c r="A302" t="inlineStr">
@@ -8001,6 +8906,9 @@
       <c r="G302" t="n">
         <v>8.010437466347517</v>
       </c>
+      <c r="H302" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="303">
       <c r="A303" t="inlineStr">
@@ -8026,6 +8934,9 @@
       <c r="G303" t="n">
         <v>8.005555366482529</v>
       </c>
+      <c r="H303" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="304">
       <c r="A304" t="inlineStr">
@@ -8051,6 +8962,9 @@
       <c r="G304" t="n">
         <v>7.871691585276367</v>
       </c>
+      <c r="H304" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="305">
       <c r="A305" t="inlineStr">
@@ -8076,6 +8990,9 @@
       <c r="G305" t="n">
         <v>7.853184088679344</v>
       </c>
+      <c r="H305" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="306">
       <c r="A306" t="inlineStr">
@@ -8101,6 +9018,9 @@
       <c r="G306" t="n">
         <v>7.830436231327608</v>
       </c>
+      <c r="H306" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="307">
       <c r="A307" t="inlineStr">
@@ -8126,6 +9046,9 @@
       <c r="G307" t="n">
         <v>7.688724255177469</v>
       </c>
+      <c r="H307" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="308">
       <c r="A308" t="inlineStr">
@@ -8151,6 +9074,9 @@
       <c r="G308" t="n">
         <v>7.639893461943316</v>
       </c>
+      <c r="H308" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="309">
       <c r="A309" t="inlineStr">
@@ -8176,6 +9102,9 @@
       <c r="G309" t="n">
         <v>7.598721050472718</v>
       </c>
+      <c r="H309" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="310">
       <c r="A310" t="inlineStr">
@@ -8201,6 +9130,9 @@
       <c r="G310" t="n">
         <v>7.590205293625987</v>
       </c>
+      <c r="H310" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="311">
       <c r="A311" t="inlineStr">
@@ -8226,6 +9158,9 @@
       <c r="G311" t="n">
         <v>7.555582808112069</v>
       </c>
+      <c r="H311" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="312">
       <c r="A312" t="inlineStr">
@@ -8251,6 +9186,9 @@
       <c r="G312" t="n">
         <v>7.555095739978952</v>
       </c>
+      <c r="H312" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="313">
       <c r="A313" t="inlineStr">
@@ -8276,6 +9214,9 @@
       <c r="G313" t="n">
         <v>7.463675867703849</v>
       </c>
+      <c r="H313" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="314">
       <c r="A314" t="inlineStr">
@@ -8301,6 +9242,9 @@
       <c r="G314" t="n">
         <v>7.343190937277654</v>
       </c>
+      <c r="H314" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="315">
       <c r="A315" t="inlineStr">
@@ -8326,6 +9270,9 @@
       <c r="G315" t="n">
         <v>7.315113602961532</v>
       </c>
+      <c r="H315" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="316">
       <c r="A316" t="inlineStr">
@@ -8351,6 +9298,9 @@
       <c r="G316" t="n">
         <v>7.284048010931799</v>
       </c>
+      <c r="H316" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="317">
       <c r="A317" t="inlineStr">
@@ -8376,6 +9326,9 @@
       <c r="G317" t="n">
         <v>7.154074746881613</v>
       </c>
+      <c r="H317" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="318">
       <c r="A318" t="inlineStr">
@@ -8401,6 +9354,9 @@
       <c r="G318" t="n">
         <v>7.146895559153989</v>
       </c>
+      <c r="H318" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="319">
       <c r="A319" t="inlineStr">
@@ -8426,6 +9382,9 @@
       <c r="G319" t="n">
         <v>7.098433018934188</v>
       </c>
+      <c r="H319" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="320">
       <c r="A320" t="inlineStr">
@@ -8451,6 +9410,9 @@
       <c r="G320" t="n">
         <v>6.942631614293369</v>
       </c>
+      <c r="H320" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="321">
       <c r="A321" t="inlineStr">
@@ -8476,6 +9438,9 @@
       <c r="G321" t="n">
         <v>6.8497040523723</v>
       </c>
+      <c r="H321" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="322">
       <c r="A322" t="inlineStr">
@@ -8501,6 +9466,9 @@
       <c r="G322" t="n">
         <v>6.823743612398276</v>
       </c>
+      <c r="H322" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="323">
       <c r="A323" t="inlineStr">
@@ -8526,6 +9494,9 @@
       <c r="G323" t="n">
         <v>6.747081212882907</v>
       </c>
+      <c r="H323" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="324">
       <c r="A324" t="inlineStr">
@@ -8551,6 +9522,9 @@
       <c r="G324" t="n">
         <v>6.714965340903255</v>
       </c>
+      <c r="H324" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="325">
       <c r="A325" t="inlineStr">
@@ -8576,6 +9550,9 @@
       <c r="G325" t="n">
         <v>6.711468204788443</v>
       </c>
+      <c r="H325" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="326">
       <c r="A326" t="inlineStr">
@@ -8601,6 +9578,9 @@
       <c r="G326" t="n">
         <v>6.701721329943903</v>
       </c>
+      <c r="H326" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="327">
       <c r="A327" t="inlineStr">
@@ -8626,6 +9606,9 @@
       <c r="G327" t="n">
         <v>6.62943406284296</v>
       </c>
+      <c r="H327" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="328">
       <c r="A328" t="inlineStr">
@@ -8651,6 +9634,9 @@
       <c r="G328" t="n">
         <v>6.625052398073511</v>
       </c>
+      <c r="H328" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="329">
       <c r="A329" t="inlineStr">
@@ -8676,6 +9662,9 @@
       <c r="G329" t="n">
         <v>6.594161614358296</v>
       </c>
+      <c r="H329" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="330">
       <c r="A330" t="inlineStr">
@@ -8701,6 +9690,9 @@
       <c r="G330" t="n">
         <v>6.491295525704483</v>
       </c>
+      <c r="H330" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="331">
       <c r="A331" t="inlineStr">
@@ -8726,6 +9718,9 @@
       <c r="G331" t="n">
         <v>6.457193754244013</v>
       </c>
+      <c r="H331" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="332">
       <c r="A332" t="inlineStr">
@@ -8751,6 +9746,9 @@
       <c r="G332" t="n">
         <v>6.421319088214929</v>
       </c>
+      <c r="H332" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="333">
       <c r="A333" t="inlineStr">
@@ -8776,6 +9774,9 @@
       <c r="G333" t="n">
         <v>6.382605525060351</v>
       </c>
+      <c r="H333" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="334">
       <c r="A334" t="inlineStr">
@@ -8801,6 +9802,9 @@
       <c r="G334" t="n">
         <v>6.360227722104557</v>
       </c>
+      <c r="H334" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="335">
       <c r="A335" t="inlineStr">
@@ -8826,6 +9830,9 @@
       <c r="G335" t="n">
         <v>6.320192132636625</v>
       </c>
+      <c r="H335" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="336">
       <c r="A336" t="inlineStr">
@@ -8851,6 +9858,9 @@
       <c r="G336" t="n">
         <v>6.237147018122816</v>
       </c>
+      <c r="H336" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="337">
       <c r="A337" t="inlineStr">
@@ -8876,6 +9886,9 @@
       <c r="G337" t="n">
         <v>6.19139959976693</v>
       </c>
+      <c r="H337" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="338">
       <c r="A338" t="inlineStr">
@@ -8901,6 +9914,9 @@
       <c r="G338" t="n">
         <v>6.170831658176943</v>
       </c>
+      <c r="H338" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="339">
       <c r="A339" t="inlineStr">
@@ -8926,6 +9942,9 @@
       <c r="G339" t="n">
         <v>6.106727192664919</v>
       </c>
+      <c r="H339" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="340">
       <c r="A340" t="inlineStr">
@@ -8951,6 +9970,9 @@
       <c r="G340" t="n">
         <v>6.031823667096926</v>
       </c>
+      <c r="H340" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="341">
       <c r="A341" t="inlineStr">
@@ -8976,6 +9998,9 @@
       <c r="G341" t="n">
         <v>5.997131613735534</v>
       </c>
+      <c r="H341" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="342">
       <c r="A342" t="inlineStr">
@@ -9001,6 +10026,9 @@
       <c r="G342" t="n">
         <v>5.995537915742794</v>
       </c>
+      <c r="H342" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="343">
       <c r="A343" t="inlineStr">
@@ -9026,6 +10054,9 @@
       <c r="G343" t="n">
         <v>5.909451032173433</v>
       </c>
+      <c r="H343" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="344">
       <c r="A344" t="inlineStr">
@@ -9051,6 +10082,9 @@
       <c r="G344" t="n">
         <v>5.872620444879751</v>
       </c>
+      <c r="H344" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="345">
       <c r="A345" t="inlineStr">
@@ -9076,6 +10110,9 @@
       <c r="G345" t="n">
         <v>5.768319540844051</v>
       </c>
+      <c r="H345" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="346">
       <c r="A346" t="inlineStr">
@@ -9101,6 +10138,9 @@
       <c r="G346" t="n">
         <v>5.648707300476386</v>
       </c>
+      <c r="H346" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="347">
       <c r="A347" t="inlineStr">
@@ -9126,6 +10166,9 @@
       <c r="G347" t="n">
         <v>5.561351037338381</v>
       </c>
+      <c r="H347" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="348">
       <c r="A348" t="inlineStr">
@@ -9151,6 +10194,9 @@
       <c r="G348" t="n">
         <v>5.544507205193293</v>
       </c>
+      <c r="H348" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="349">
       <c r="A349" t="inlineStr">
@@ -9176,6 +10222,9 @@
       <c r="G349" t="n">
         <v>5.517412929430772</v>
       </c>
+      <c r="H349" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="350">
       <c r="A350" t="inlineStr">
@@ -9201,6 +10250,9 @@
       <c r="G350" t="n">
         <v>5.506219315702235</v>
       </c>
+      <c r="H350" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="351">
       <c r="A351" t="inlineStr">
@@ -9226,6 +10278,9 @@
       <c r="G351" t="n">
         <v>5.398353118964666</v>
       </c>
+      <c r="H351" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="352">
       <c r="A352" t="inlineStr">
@@ -9251,6 +10306,9 @@
       <c r="G352" t="n">
         <v>5.321669324521422</v>
       </c>
+      <c r="H352" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="353">
       <c r="A353" t="inlineStr">
@@ -9276,6 +10334,9 @@
       <c r="G353" t="n">
         <v>5.287343167623108</v>
       </c>
+      <c r="H353" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="354">
       <c r="A354" t="inlineStr">
@@ -9301,6 +10362,9 @@
       <c r="G354" t="n">
         <v>5.229560391400217</v>
       </c>
+      <c r="H354" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="355">
       <c r="A355" t="inlineStr">
@@ -9326,6 +10390,9 @@
       <c r="G355" t="n">
         <v>5.223722873586468</v>
       </c>
+      <c r="H355" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="356">
       <c r="A356" t="inlineStr">
@@ -9351,6 +10418,9 @@
       <c r="G356" t="n">
         <v>5.064387528364596</v>
       </c>
+      <c r="H356" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="357">
       <c r="A357" t="inlineStr">
@@ -9376,6 +10446,9 @@
       <c r="G357" t="n">
         <v>5.041930012268017</v>
       </c>
+      <c r="H357" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="358">
       <c r="A358" t="inlineStr">
@@ -9401,6 +10474,9 @@
       <c r="G358" t="n">
         <v>4.881150818330119</v>
       </c>
+      <c r="H358" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="359">
       <c r="A359" t="inlineStr">
@@ -9426,6 +10502,9 @@
       <c r="G359" t="n">
         <v>4.720694217878125</v>
       </c>
+      <c r="H359" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="360">
       <c r="A360" t="inlineStr">
@@ -9451,6 +10530,9 @@
       <c r="G360" t="n">
         <v>4.707531507636279</v>
       </c>
+      <c r="H360" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="361">
       <c r="A361" t="inlineStr">
@@ -9476,6 +10558,9 @@
       <c r="G361" t="n">
         <v>4.703519900234774</v>
       </c>
+      <c r="H361" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="362">
       <c r="A362" t="inlineStr">
@@ -9501,6 +10586,9 @@
       <c r="G362" t="n">
         <v>4.619374656149435</v>
       </c>
+      <c r="H362" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="363">
       <c r="A363" t="inlineStr">
@@ -9526,6 +10614,9 @@
       <c r="G363" t="n">
         <v>4.615239601394896</v>
       </c>
+      <c r="H363" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="364">
       <c r="A364" t="inlineStr">
@@ -9551,6 +10642,9 @@
       <c r="G364" t="n">
         <v>4.517260144710548</v>
       </c>
+      <c r="H364" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="365">
       <c r="A365" t="inlineStr">
@@ -9576,6 +10670,9 @@
       <c r="G365" t="n">
         <v>4.50871534009222</v>
       </c>
+      <c r="H365" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="366">
       <c r="A366" t="inlineStr">
@@ -9601,6 +10698,9 @@
       <c r="G366" t="n">
         <v>4.313936242030343</v>
       </c>
+      <c r="H366" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="367">
       <c r="A367" t="inlineStr">
@@ -9626,6 +10726,9 @@
       <c r="G367" t="n">
         <v>4.27345154761554</v>
       </c>
+      <c r="H367" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="368">
       <c r="A368" t="inlineStr">
@@ -9651,6 +10754,9 @@
       <c r="G368" t="n">
         <v>4.27245220378628</v>
       </c>
+      <c r="H368" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="369">
       <c r="A369" t="inlineStr">
@@ -9676,6 +10782,9 @@
       <c r="G369" t="n">
         <v>4.165807415890609</v>
       </c>
+      <c r="H369" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="370">
       <c r="A370" t="inlineStr">
@@ -9701,6 +10810,9 @@
       <c r="G370" t="n">
         <v>3.906570721462156</v>
       </c>
+      <c r="H370" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="371">
       <c r="A371" t="inlineStr">
@@ -9726,6 +10838,9 @@
       <c r="G371" t="n">
         <v>3.88052157835617</v>
       </c>
+      <c r="H371" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="372">
       <c r="A372" t="inlineStr">
@@ -9751,6 +10866,9 @@
       <c r="G372" t="n">
         <v>3.714774909150434</v>
       </c>
+      <c r="H372" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="373">
       <c r="A373" t="inlineStr">
@@ -9776,6 +10894,9 @@
       <c r="G373" t="n">
         <v>3.697502930885809</v>
       </c>
+      <c r="H373" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="374">
       <c r="A374" t="inlineStr">
@@ -9801,6 +10922,9 @@
       <c r="G374" t="n">
         <v>3.670023502062919</v>
       </c>
+      <c r="H374" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="375">
       <c r="A375" t="inlineStr">
@@ -9826,6 +10950,9 @@
       <c r="G375" t="n">
         <v>3.266231710827213</v>
       </c>
+      <c r="H375" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="376">
       <c r="A376" t="inlineStr">
@@ -9851,6 +10978,9 @@
       <c r="G376" t="n">
         <v>3.186295032435734</v>
       </c>
+      <c r="H376" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="377">
       <c r="A377" t="inlineStr">
@@ -9876,6 +11006,9 @@
       <c r="G377" t="n">
         <v>3.134992791250899</v>
       </c>
+      <c r="H377" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="378">
       <c r="A378" t="inlineStr">
@@ -9901,6 +11034,9 @@
       <c r="G378" t="n">
         <v>3.044343019262881</v>
       </c>
+      <c r="H378" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="379">
       <c r="A379" t="inlineStr">
@@ -9926,6 +11062,9 @@
       <c r="G379" t="n">
         <v>2.954722489606652</v>
       </c>
+      <c r="H379" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="380">
       <c r="A380" t="inlineStr">
@@ -9951,6 +11090,9 @@
       <c r="G380" t="n">
         <v>2.944644177504548</v>
       </c>
+      <c r="H380" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="381">
       <c r="A381" t="inlineStr">
@@ -9976,6 +11118,9 @@
       <c r="G381" t="n">
         <v>2.447173923766281</v>
       </c>
+      <c r="H381" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="382">
       <c r="A382" t="inlineStr">
@@ -10001,6 +11146,9 @@
       <c r="G382" t="n">
         <v>2.390166610288636</v>
       </c>
+      <c r="H382" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="383">
       <c r="A383" t="inlineStr">
@@ -10026,6 +11174,9 @@
       <c r="G383" t="n">
         <v>2.325205670123101</v>
       </c>
+      <c r="H383" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="384">
       <c r="A384" t="inlineStr">
@@ -10051,6 +11202,9 @@
       <c r="G384" t="n">
         <v>2.319010572904426</v>
       </c>
+      <c r="H384" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="385">
       <c r="A385" t="inlineStr">
@@ -10076,6 +11230,9 @@
       <c r="G385" t="n">
         <v>2.317932719603999</v>
       </c>
+      <c r="H385" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="386">
       <c r="A386" t="inlineStr">
@@ -10101,6 +11258,9 @@
       <c r="G386" t="n">
         <v>2.315740903737122</v>
       </c>
+      <c r="H386" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="387">
       <c r="A387" t="inlineStr">
@@ -10126,6 +11286,9 @@
       <c r="G387" t="n">
         <v>2.29413705852976</v>
       </c>
+      <c r="H387" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="388">
       <c r="A388" t="inlineStr">
@@ -10151,6 +11314,9 @@
       <c r="G388" t="n">
         <v>2.284933649468034</v>
       </c>
+      <c r="H388" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="389">
       <c r="A389" t="inlineStr">
@@ -10176,6 +11342,9 @@
       <c r="G389" t="n">
         <v>2.263796074909136</v>
       </c>
+      <c r="H389" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="390">
       <c r="A390" t="inlineStr">
@@ -10201,6 +11370,9 @@
       <c r="G390" t="n">
         <v>2.243773707055322</v>
       </c>
+      <c r="H390" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="391">
       <c r="A391" t="inlineStr">
@@ -10226,6 +11398,9 @@
       <c r="G391" t="n">
         <v>2.241644814335632</v>
       </c>
+      <c r="H391" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="392">
       <c r="A392" t="inlineStr">
@@ -10251,6 +11426,9 @@
       <c r="G392" t="n">
         <v>2.192121279362655</v>
       </c>
+      <c r="H392" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="393">
       <c r="A393" t="inlineStr">
@@ -10276,6 +11454,9 @@
       <c r="G393" t="n">
         <v>2.184386010591988</v>
       </c>
+      <c r="H393" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="394">
       <c r="A394" t="inlineStr">
@@ -10301,6 +11482,9 @@
       <c r="G394" t="n">
         <v>2.170877444079967</v>
       </c>
+      <c r="H394" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="395">
       <c r="A395" t="inlineStr">
@@ -10326,6 +11510,9 @@
       <c r="G395" t="n">
         <v>2.165737209254587</v>
       </c>
+      <c r="H395" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="396">
       <c r="A396" t="inlineStr">
@@ -10351,6 +11538,9 @@
       <c r="G396" t="n">
         <v>2.117989722418755</v>
       </c>
+      <c r="H396" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="397">
       <c r="A397" t="inlineStr">
@@ -10376,6 +11566,9 @@
       <c r="G397" t="n">
         <v>2.117509935180234</v>
       </c>
+      <c r="H397" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="398">
       <c r="A398" t="inlineStr">
@@ -10401,6 +11594,9 @@
       <c r="G398" t="n">
         <v>2.073136996688747</v>
       </c>
+      <c r="H398" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="399">
       <c r="A399" t="inlineStr">
@@ -10426,6 +11622,9 @@
       <c r="G399" t="n">
         <v>1.969176647004699</v>
       </c>
+      <c r="H399" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="400">
       <c r="A400" t="inlineStr">
@@ -10451,6 +11650,9 @@
       <c r="G400" t="n">
         <v>1.961873753103412</v>
       </c>
+      <c r="H400" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="401">
       <c r="A401" t="inlineStr">
@@ -10476,6 +11678,9 @@
       <c r="G401" t="n">
         <v>0</v>
       </c>
+      <c r="H401" t="n">
+        <v>16569</v>
+      </c>
     </row>
     <row r="402">
       <c r="A402" t="inlineStr">
@@ -10501,6 +11706,9 @@
       <c r="G402" t="n">
         <v>0</v>
       </c>
+      <c r="H402" t="n">
+        <v>1152</v>
+      </c>
     </row>
     <row r="403">
       <c r="A403" t="inlineStr">
@@ -10526,6 +11734,9 @@
       <c r="G403" t="n">
         <v>0</v>
       </c>
+      <c r="H403" t="n">
+        <v>1051</v>
+      </c>
     </row>
     <row r="404">
       <c r="A404" t="inlineStr">
@@ -10549,6 +11760,9 @@
         <v>5792.96</v>
       </c>
       <c r="G404" t="n">
+        <v>0</v>
+      </c>
+      <c r="H404" t="n">
         <v>0</v>
       </c>
     </row>
@@ -38692,7 +39906,7 @@
         <v>0.02310694271200725</v>
       </c>
       <c r="E2" t="n">
-        <v>1079.108283410909</v>
+        <v>1091.966828865455</v>
       </c>
     </row>
     <row r="3">

</xml_diff>